<commit_message>
#24: writing shifts. Need a cut through two days.
</commit_message>
<xml_diff>
--- a/data/roster/template_for_roster_results.xlsx
+++ b/data/roster/template_for_roster_results.xlsx
@@ -417,7 +417,7 @@
       <charset val="186"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial1"/>
       <family val="0"/>
@@ -2625,8 +2625,8 @@
   </sheetPr>
   <dimension ref="A2:AR603"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP114" activeCellId="0" sqref="AP114"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10:AJ111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26143,7 +26143,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="1" sqref="F10:AJ111 D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26166,7 +26166,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:AJ111 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26189,7 +26189,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:AJ111 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26212,7 +26212,7 @@
   <dimension ref="A1:CB127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="F10:AJ111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36910,7 +36910,7 @@
       <c r="B123" s="254"/>
       <c r="C123" s="269" t="n">
         <f aca="true">NOW()</f>
-        <v>45605.7591637938</v>
+        <v>45608.125068148</v>
       </c>
       <c r="D123" s="269"/>
       <c r="E123" s="254"/>
@@ -37518,7 +37518,7 @@
   <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F10:AJ111 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41547,7 +41547,7 @@
   <dimension ref="C6:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="F10:AJ111 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
#27: fixed excel template and hours per day output.
</commit_message>
<xml_diff>
--- a/data/roster/template_for_roster_results.xlsx
+++ b/data/roster/template_for_roster_results.xlsx
@@ -8,16 +8,16 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Darbo grafikas" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="belekoks" sheetId="2" state="hidden" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="4" state="hidden" r:id="rId6"/>
-    <sheet name="Tabelis" sheetId="5" state="hidden" r:id="rId7"/>
-    <sheet name="Tarpine" sheetId="6" state="hidden" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId9"/>
+    <sheet name="Darbo grafikas" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="belekoks" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Tabelis" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="Tarpine" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="4" name="Z_3A6C2238_6F2F_4B16_9EF0_DF591EBA9496_.wvu.Rows" vbProcedure="false">Tabelis!$13:$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="Z_3A6C2238_6F2F_4B16_9EF0_DF591EBA9496_.wvu.Rows" vbProcedure="false">Tabelis!$13:$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -363,14 +363,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="186"/>
@@ -418,7 +418,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial1"/>
       <family val="0"/>
       <charset val="186"/>
@@ -716,7 +716,7 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="186"/>
@@ -737,7 +737,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
@@ -2349,7 +2349,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2443,207 +2443,32 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1f497d"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="eeece1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A2:AR603"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10:AJ111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="6" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="14" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="5.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="16" style="1" width="5.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="5.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="40" style="1" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="40" style="1" width="9.66"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26126,8 +25951,8 @@
     <mergeCell ref="AJ248:AJ249"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.2" right="0.2" top="0.309722222222222" bottom="0.240277777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.2" right="0.2" top="0.309722222222222" bottom="0.240277777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -26136,21 +25961,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="1" sqref="F10:AJ111 D41"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -26159,21 +25984,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:AJ111 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -26182,21 +26007,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:AJ111 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -26205,36 +26030,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CB127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="F10:AJ111"/>
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="66" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="66" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="66" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="66" width="14.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="7" style="1" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="67" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="67" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="67" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="67" width="3.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="67" width="3.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="67" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="67" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="67" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="67" width="3.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="67" width="4.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="76" style="67" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="67" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="67" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="67" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="67" width="3.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36910,7 +36735,7 @@
       <c r="B123" s="254"/>
       <c r="C123" s="269" t="n">
         <f aca="true">NOW()</f>
-        <v>45608.125068148</v>
+        <v>45621.4114329427</v>
       </c>
       <c r="D123" s="269"/>
       <c r="E123" s="254"/>
@@ -37501,8 +37326,8 @@
     <mergeCell ref="C123:D123"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="0.0395833333333333" bottom="0.0395833333333333" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="44" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.0395833333333333" bottom="0.0395833333333333" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="44" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -37511,20 +37336,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F10:AJ111 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="2" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="2" style="1" width="5.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41530,8 +41355,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -41540,17 +41365,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="C6:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="F10:AJ111 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="60"/>
@@ -41591,8 +41416,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
#27: Assigned hours sums written to results file.
</commit_message>
<xml_diff>
--- a/data/roster/template_for_roster_results.xlsx
+++ b/data/roster/template_for_roster_results.xlsx
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Darbo dienų</t>
   </si>
   <si>
-    <t xml:space="preserve">Darbo valan-dų</t>
+    <t xml:space="preserve">Darbo valandų priskirta</t>
   </si>
   <si>
     <t xml:space="preserve">Darbo valandų per mėnesį</t>
@@ -2451,14 +2451,14 @@
   <dimension ref="A2:AR603"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="AL10" activeCellId="0" sqref="AL10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="5.83"/>
@@ -25971,7 +25971,7 @@
       <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -25994,7 +25994,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -26017,7 +26017,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -26040,26 +26040,26 @@
       <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="66" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="66" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="66" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="66" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="7" style="1" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="67" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="67" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="67" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="67" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="67" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="67" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="67" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="67" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="67" width="4.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="76" style="67" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="67" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="67" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="67" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="67" width="3.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36735,7 +36735,7 @@
       <c r="B123" s="254"/>
       <c r="C123" s="269" t="n">
         <f aca="true">NOW()</f>
-        <v>45621.4114329427</v>
+        <v>45621.6237154102</v>
       </c>
       <c r="D123" s="269"/>
       <c r="E123" s="254"/>
@@ -37346,7 +37346,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="2" style="1" width="5.01"/>
@@ -41375,7 +41375,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="60"/>

</xml_diff>